<commit_message>
Adding another test point
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestEvent/ActivityData/ActivityData_FEB3.xlsx
+++ b/src/test/resources/TestDriver/TestEvent/ActivityData/ActivityData_FEB3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestEvent\ActivityData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D26643-F5DC-4AD8-9A2E-44B1DFC63EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A05C76-10B1-4F53-9BA1-BFD68D6F88E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="4635" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
   <si>
     <t>Postingdate</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>actual_360</t>
-  </si>
-  <si>
-    <t>current</t>
   </si>
   <si>
     <t>Sporting Goods and Outdoors</t>
@@ -591,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048572"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -687,11 +684,11 @@
       <c r="K2" s="11">
         <v>100000</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="11">
+        <v>4</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="N2" s="16">
         <f>A2</f>
@@ -730,7 +727,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="11">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I3" s="16">
         <v>44592</v>
@@ -741,11 +738,11 @@
       <c r="K3" s="11">
         <v>150000</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="11">
+        <v>4</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="N3" s="16">
         <f>A3</f>
@@ -788,7 +785,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>